<commit_message>
Todo funcional, se agregó el comparador de columnas y el comparador de Header con tipo de variable
</commit_message>
<xml_diff>
--- a/project-a/src/bd/bd.xlsx
+++ b/project-a/src/bd/bd.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniecja\Downloads\Echava\Code\project-a\project-a\src\bd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniecja\Downloads\Echava\Code\Git\astro_vs_spring\project-a\src\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5FC81F-C450-41D6-89C0-B80D08B8F213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4380BEF9-C89D-4A7A-8547-A8C155AC32CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{B39321D7-4FD5-4A10-8A62-B474F467BC99}"/>
   </bookViews>
@@ -436,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4E5CD9-2F0B-4F97-B67C-012DB45ECAFB}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,7 +447,7 @@
     <col min="2" max="2" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,8 +466,9 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -487,7 +488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -507,7 +508,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -527,7 +528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -547,7 +548,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -567,7 +568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -587,7 +588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -607,7 +608,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -627,7 +628,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -647,7 +648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -667,7 +668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -687,7 +688,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -707,7 +708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -727,7 +728,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -747,7 +748,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>